<commit_message>
Add info about planning horizon
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/14-tastks109/14-tastks109.xlsx
+++ b/ampl-data-input-excel/14-tastks109/14-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -5775,8 +5775,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6030,7 +6030,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6082,7 +6082,8 @@
         <v>45658</v>
       </c>
       <c r="F2" s="14" t="n">
-        <v>46053</v>
+        <f aca="false">E2+20</f>
+        <v>45678</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>0.6</v>
@@ -6211,7 +6212,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6282,7 +6283,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -16325,8 +16326,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>